<commit_message>
adding data up to 7th
</commit_message>
<xml_diff>
--- a/full_time_work_prop.xlsx
+++ b/full_time_work_prop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Alaska</t>
   </si>
@@ -624,6 +624,39 @@
   <si>
     <t>26 06 2020</t>
   </si>
+  <si>
+    <t>27 06 2020</t>
+  </si>
+  <si>
+    <t>28 06 2020</t>
+  </si>
+  <si>
+    <t>29 06 2020</t>
+  </si>
+  <si>
+    <t>30 06 2020</t>
+  </si>
+  <si>
+    <t>01 07 2020</t>
+  </si>
+  <si>
+    <t>02 07 2020</t>
+  </si>
+  <si>
+    <t>03 07 2020</t>
+  </si>
+  <si>
+    <t>04 07 2020</t>
+  </si>
+  <si>
+    <t>05 07 2020</t>
+  </si>
+  <si>
+    <t>06 07 2020</t>
+  </si>
+  <si>
+    <t>07 07 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -954,7 +987,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE148"/>
+  <dimension ref="A1:BE159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12388,6 +12421,9 @@
       <c r="D67">
         <v>0.047268808604219</v>
       </c>
+      <c r="E67">
+        <v>0.16666666666667</v>
+      </c>
       <c r="F67">
         <v>0.040916434586717</v>
       </c>
@@ -12558,6 +12594,9 @@
       <c r="D68">
         <v>0.045107135389434</v>
       </c>
+      <c r="E68">
+        <v>0.11111111111111</v>
+      </c>
       <c r="F68">
         <v>0.035223704761174</v>
       </c>
@@ -24619,50 +24658,2745 @@
       <c r="A139" t="s">
         <v>193</v>
       </c>
+      <c r="B139">
+        <v>0.052795408790617</v>
+      </c>
+      <c r="C139">
+        <v>0.06561874373694999</v>
+      </c>
+      <c r="D139">
+        <v>0.049072986882549</v>
+      </c>
+      <c r="F139">
+        <v>0.042815433699982</v>
+      </c>
+      <c r="G139">
+        <v>0.047549620063945</v>
+      </c>
+      <c r="H139">
+        <v>0.047547212656227</v>
+      </c>
+      <c r="I139">
+        <v>0.040311441109748</v>
+      </c>
+      <c r="J139">
+        <v>0.038852021040307</v>
+      </c>
+      <c r="K139">
+        <v>0.040767130780322</v>
+      </c>
+      <c r="L139">
+        <v>0.044913236860644</v>
+      </c>
+      <c r="M139">
+        <v>0.04616701071513</v>
+      </c>
+      <c r="N139">
+        <v>0.052487067371616</v>
+      </c>
+      <c r="O139">
+        <v>0.030513524312905</v>
+      </c>
+      <c r="P139">
+        <v>0.052732378442493</v>
+      </c>
+      <c r="Q139">
+        <v>0.055409670097008</v>
+      </c>
+      <c r="R139">
+        <v>0.047575768859418</v>
+      </c>
+      <c r="S139">
+        <v>0.050124583763374</v>
+      </c>
+      <c r="T139">
+        <v>0.053251763920884</v>
+      </c>
+      <c r="U139">
+        <v>0.050965740892454</v>
+      </c>
+      <c r="V139">
+        <v>0.058250255387749</v>
+      </c>
+      <c r="W139">
+        <v>0.05075694167054</v>
+      </c>
+      <c r="X139">
+        <v>0.047287498405627</v>
+      </c>
+      <c r="Y139">
+        <v>0.05602317216</v>
+      </c>
+      <c r="Z139">
+        <v>0.051506196674293</v>
+      </c>
+      <c r="AA139">
+        <v>0.04695010177658</v>
+      </c>
+      <c r="AB139">
+        <v>0.05463477385885</v>
+      </c>
+      <c r="AC139">
+        <v>0.15343040797586</v>
+      </c>
+      <c r="AD139">
+        <v>0.05466554323954</v>
+      </c>
+      <c r="AE139">
+        <v>0.063169652421751</v>
+      </c>
+      <c r="AF139">
+        <v>0.04370543928655</v>
+      </c>
+      <c r="AG139">
+        <v>0.041672741218108</v>
+      </c>
+      <c r="AH139">
+        <v>0.052646307929367</v>
+      </c>
+      <c r="AI139">
+        <v>0.054402573878368</v>
+      </c>
+      <c r="AJ139">
+        <v>0.045630855341789</v>
+      </c>
+      <c r="AK139">
+        <v>0.053187078922726</v>
+      </c>
+      <c r="AL139">
+        <v>0.048259207077419</v>
+      </c>
+      <c r="AM139">
+        <v>0.046452156821822</v>
+      </c>
+      <c r="AN139">
+        <v>0.041704584616902</v>
+      </c>
+      <c r="AO139">
+        <v>0.04443601237543</v>
+      </c>
+      <c r="AP139">
+        <v>0.040361074918062</v>
+      </c>
+      <c r="AQ139">
+        <v>0.042655685708575</v>
+      </c>
+      <c r="AR139">
+        <v>0.045627894855103</v>
+      </c>
+      <c r="AS139">
+        <v>0.043743723863863</v>
+      </c>
+      <c r="AT139">
+        <v>0.048441332498619</v>
+      </c>
+      <c r="AU139">
+        <v>0.046088278477154</v>
+      </c>
+      <c r="AV139">
+        <v>0.047264641560706</v>
+      </c>
+      <c r="AW139">
+        <v>0.044770032259484</v>
+      </c>
+      <c r="AX139">
+        <v>0.053919619219998</v>
+      </c>
+      <c r="AY139">
+        <v>0.045379725995676</v>
+      </c>
+      <c r="AZ139">
+        <v>0.084755365713319</v>
+      </c>
+      <c r="BA139">
+        <v>0.051107137025188</v>
+      </c>
+      <c r="BB139">
+        <v>0.042216130065921</v>
+      </c>
+      <c r="BC139">
+        <v>0.045570857822901</v>
+      </c>
+      <c r="BD139">
+        <v>0.048171935390025</v>
+      </c>
+      <c r="BE139">
+        <v>0.042190237794212</v>
+      </c>
     </row>
     <row r="140" spans="1:57">
       <c r="A140" t="s">
         <v>194</v>
       </c>
+      <c r="B140">
+        <v>0.047233526597902</v>
+      </c>
+      <c r="C140">
+        <v>0.04989733676006</v>
+      </c>
+      <c r="D140">
+        <v>0.040807059351874</v>
+      </c>
+      <c r="F140">
+        <v>0.036502722527791</v>
+      </c>
+      <c r="G140">
+        <v>0.04996184627656</v>
+      </c>
+      <c r="H140">
+        <v>0.053252665674383</v>
+      </c>
+      <c r="I140">
+        <v>0.047858470576585</v>
+      </c>
+      <c r="J140">
+        <v>0.044215209598088</v>
+      </c>
+      <c r="K140">
+        <v>0.048682774590613</v>
+      </c>
+      <c r="L140">
+        <v>0.049181470461762</v>
+      </c>
+      <c r="M140">
+        <v>0.046020688154221</v>
+      </c>
+      <c r="N140">
+        <v>0.063491707648047</v>
+      </c>
+      <c r="O140">
+        <v>0.030312883212578</v>
+      </c>
+      <c r="P140">
+        <v>0.048588898438488</v>
+      </c>
+      <c r="Q140">
+        <v>0.056637466517113</v>
+      </c>
+      <c r="R140">
+        <v>0.045724015498408</v>
+      </c>
+      <c r="S140">
+        <v>0.048046181267075</v>
+      </c>
+      <c r="T140">
+        <v>0.047809605970067</v>
+      </c>
+      <c r="U140">
+        <v>0.048634074565594</v>
+      </c>
+      <c r="V140">
+        <v>0.055844504102557</v>
+      </c>
+      <c r="W140">
+        <v>0.047628868716206</v>
+      </c>
+      <c r="X140">
+        <v>0.04423939439937</v>
+      </c>
+      <c r="Y140">
+        <v>0.052317820037331</v>
+      </c>
+      <c r="Z140">
+        <v>0.049390696815707</v>
+      </c>
+      <c r="AA140">
+        <v>0.045587258409102</v>
+      </c>
+      <c r="AB140">
+        <v>0.052042990836652</v>
+      </c>
+      <c r="AC140">
+        <v>0.13275887530273</v>
+      </c>
+      <c r="AD140">
+        <v>0.052593434459539</v>
+      </c>
+      <c r="AE140">
+        <v>0.059435025514648</v>
+      </c>
+      <c r="AF140">
+        <v>0.041924477690026</v>
+      </c>
+      <c r="AG140">
+        <v>0.041965345613</v>
+      </c>
+      <c r="AH140">
+        <v>0.048002596990173</v>
+      </c>
+      <c r="AI140">
+        <v>0.046738643964905</v>
+      </c>
+      <c r="AJ140">
+        <v>0.040287378896615</v>
+      </c>
+      <c r="AK140">
+        <v>0.047463854105761</v>
+      </c>
+      <c r="AL140">
+        <v>0.046723680812461</v>
+      </c>
+      <c r="AM140">
+        <v>0.041693707955021</v>
+      </c>
+      <c r="AN140">
+        <v>0.041838050068461</v>
+      </c>
+      <c r="AO140">
+        <v>0.044577653140272</v>
+      </c>
+      <c r="AP140">
+        <v>0.042454060389047</v>
+      </c>
+      <c r="AQ140">
+        <v>0.043428889826012</v>
+      </c>
+      <c r="AR140">
+        <v>0.053789831305432</v>
+      </c>
+      <c r="AS140">
+        <v>0.045322293094634</v>
+      </c>
+      <c r="AT140">
+        <v>0.047449216677586</v>
+      </c>
+      <c r="AU140">
+        <v>0.048023414509765</v>
+      </c>
+      <c r="AV140">
+        <v>0.047446145636777</v>
+      </c>
+      <c r="AW140">
+        <v>0.04534007398687</v>
+      </c>
+      <c r="AX140">
+        <v>0.055945537181735</v>
+      </c>
+      <c r="AY140">
+        <v>0.047826639886274</v>
+      </c>
+      <c r="AZ140">
+        <v>0.08242715838220301</v>
+      </c>
+      <c r="BA140">
+        <v>0.058358320915999</v>
+      </c>
+      <c r="BB140">
+        <v>0.046892665258717</v>
+      </c>
+      <c r="BC140">
+        <v>0.050808313068178</v>
+      </c>
+      <c r="BD140">
+        <v>0.055697887452677</v>
+      </c>
+      <c r="BE140">
+        <v>0.050774381948429</v>
+      </c>
     </row>
     <row r="141" spans="1:57">
       <c r="A141" t="s">
         <v>195</v>
       </c>
+      <c r="B141">
+        <v>0.038471630001911</v>
+      </c>
+      <c r="C141">
+        <v>0.034175858335496</v>
+      </c>
+      <c r="D141">
+        <v>0.030186962744477</v>
+      </c>
+      <c r="F141">
+        <v>0.029814188597334</v>
+      </c>
+      <c r="G141">
+        <v>0.050034683267055</v>
+      </c>
+      <c r="H141">
+        <v>0.04939114886945</v>
+      </c>
+      <c r="I141">
+        <v>0.041341499781582</v>
+      </c>
+      <c r="J141">
+        <v>0.043363008968932</v>
+      </c>
+      <c r="K141">
+        <v>0.039617517533326</v>
+      </c>
+      <c r="L141">
+        <v>0.041234772294542</v>
+      </c>
+      <c r="M141">
+        <v>0.038216912088015</v>
+      </c>
+      <c r="N141">
+        <v>0.05253756739228</v>
+      </c>
+      <c r="O141">
+        <v>0.030580780451772</v>
+      </c>
+      <c r="P141">
+        <v>0.046827876165053</v>
+      </c>
+      <c r="Q141">
+        <v>0.046231005628</v>
+      </c>
+      <c r="R141">
+        <v>0.041591129080644</v>
+      </c>
+      <c r="S141">
+        <v>0.045523112771073</v>
+      </c>
+      <c r="T141">
+        <v>0.045774252285723</v>
+      </c>
+      <c r="U141">
+        <v>0.046467016623671</v>
+      </c>
+      <c r="V141">
+        <v>0.051097606055246</v>
+      </c>
+      <c r="W141">
+        <v>0.048071639345568</v>
+      </c>
+      <c r="X141">
+        <v>0.043079129877674</v>
+      </c>
+      <c r="Y141">
+        <v>0.050366177747986</v>
+      </c>
+      <c r="Z141">
+        <v>0.045640742685815</v>
+      </c>
+      <c r="AA141">
+        <v>0.040219549314878</v>
+      </c>
+      <c r="AB141">
+        <v>0.046134203743075</v>
+      </c>
+      <c r="AC141">
+        <v>0.13722943722944</v>
+      </c>
+      <c r="AD141">
+        <v>0.046536673199264</v>
+      </c>
+      <c r="AE141">
+        <v>0.054471213786552</v>
+      </c>
+      <c r="AF141">
+        <v>0.039302767853883</v>
+      </c>
+      <c r="AG141">
+        <v>0.040741628657113</v>
+      </c>
+      <c r="AH141">
+        <v>0.044071104575663</v>
+      </c>
+      <c r="AI141">
+        <v>0.047014464693769</v>
+      </c>
+      <c r="AJ141">
+        <v>0.040624640555385</v>
+      </c>
+      <c r="AK141">
+        <v>0.048618617574274</v>
+      </c>
+      <c r="AL141">
+        <v>0.044130421999878</v>
+      </c>
+      <c r="AM141">
+        <v>0.044483046699828</v>
+      </c>
+      <c r="AN141">
+        <v>0.043600399573083</v>
+      </c>
+      <c r="AO141">
+        <v>0.045215394109773</v>
+      </c>
+      <c r="AP141">
+        <v>0.045880644667387</v>
+      </c>
+      <c r="AQ141">
+        <v>0.047308982150658</v>
+      </c>
+      <c r="AR141">
+        <v>0.049778978893564</v>
+      </c>
+      <c r="AS141">
+        <v>0.053192535691057</v>
+      </c>
+      <c r="AT141">
+        <v>0.043874552114178</v>
+      </c>
+      <c r="AU141">
+        <v>0.049671135834506</v>
+      </c>
+      <c r="AV141">
+        <v>0.04440450991379</v>
+      </c>
+      <c r="AW141">
+        <v>0.037624322221656</v>
+      </c>
+      <c r="AX141">
+        <v>0.047616268074933</v>
+      </c>
+      <c r="AY141">
+        <v>0.038815807915268</v>
+      </c>
+      <c r="AZ141">
+        <v>0.08222994228200101</v>
+      </c>
+      <c r="BA141">
+        <v>0.054207136822485</v>
+      </c>
+      <c r="BB141">
+        <v>0.039195846905841</v>
+      </c>
+      <c r="BC141">
+        <v>0.042425594278626</v>
+      </c>
+      <c r="BD141">
+        <v>0.04350544445152</v>
+      </c>
+      <c r="BE141">
+        <v>0.043072780470675</v>
+      </c>
     </row>
     <row r="142" spans="1:57">
       <c r="A142" t="s">
         <v>196</v>
       </c>
+      <c r="B142">
+        <v>0.048813329991361</v>
+      </c>
+      <c r="C142">
+        <v>0.025115232303731</v>
+      </c>
+      <c r="D142">
+        <v>0.027138982419354</v>
+      </c>
+      <c r="F142">
+        <v>0.037504151667556</v>
+      </c>
+      <c r="G142">
+        <v>0.035240578998852</v>
+      </c>
+      <c r="H142">
+        <v>0.037478596218665</v>
+      </c>
+      <c r="I142">
+        <v>0.032082780941499</v>
+      </c>
+      <c r="J142">
+        <v>0.042710880529554</v>
+      </c>
+      <c r="K142">
+        <v>0.031921817282282</v>
+      </c>
+      <c r="L142">
+        <v>0.028707042371674</v>
+      </c>
+      <c r="M142">
+        <v>0.026587232918609</v>
+      </c>
+      <c r="N142">
+        <v>0.051646123002522</v>
+      </c>
+      <c r="O142">
+        <v>0.027600584095319</v>
+      </c>
+      <c r="P142">
+        <v>0.026872666486127</v>
+      </c>
+      <c r="Q142">
+        <v>0.03566326271313</v>
+      </c>
+      <c r="R142">
+        <v>0.030543159687533</v>
+      </c>
+      <c r="S142">
+        <v>0.027620909549587</v>
+      </c>
+      <c r="T142">
+        <v>0.026306227529155</v>
+      </c>
+      <c r="U142">
+        <v>0.026724195587786</v>
+      </c>
+      <c r="V142">
+        <v>0.030274549859448</v>
+      </c>
+      <c r="W142">
+        <v>0.033252090671173</v>
+      </c>
+      <c r="X142">
+        <v>0.026803903256271</v>
+      </c>
+      <c r="Y142">
+        <v>0.035747333527053</v>
+      </c>
+      <c r="Z142">
+        <v>0.029254305364031</v>
+      </c>
+      <c r="AA142">
+        <v>0.026987470759085</v>
+      </c>
+      <c r="AB142">
+        <v>0.026777031288336</v>
+      </c>
+      <c r="AC142">
+        <v>0.13339738964739</v>
+      </c>
+      <c r="AD142">
+        <v>0.026350985524799</v>
+      </c>
+      <c r="AE142">
+        <v>0.041892497940324</v>
+      </c>
+      <c r="AF142">
+        <v>0.026851219342544</v>
+      </c>
+      <c r="AG142">
+        <v>0.030105441302848</v>
+      </c>
+      <c r="AH142">
+        <v>0.025428243452927</v>
+      </c>
+      <c r="AI142">
+        <v>0.028835932165533</v>
+      </c>
+      <c r="AJ142">
+        <v>0.028756336777024</v>
+      </c>
+      <c r="AK142">
+        <v>0.041793272861345</v>
+      </c>
+      <c r="AL142">
+        <v>0.033548316762908</v>
+      </c>
+      <c r="AM142">
+        <v>0.037202068621166</v>
+      </c>
+      <c r="AN142">
+        <v>0.03144532103561</v>
+      </c>
+      <c r="AO142">
+        <v>0.02842016046374</v>
+      </c>
+      <c r="AP142">
+        <v>0.036572406778665</v>
+      </c>
+      <c r="AQ142">
+        <v>0.035567025339329</v>
+      </c>
+      <c r="AR142">
+        <v>0.039085937072923</v>
+      </c>
+      <c r="AS142">
+        <v>0.044113820923753</v>
+      </c>
+      <c r="AT142">
+        <v>0.030497947961826</v>
+      </c>
+      <c r="AU142">
+        <v>0.037579763902157</v>
+      </c>
+      <c r="AV142">
+        <v>0.030492442567464</v>
+      </c>
+      <c r="AW142">
+        <v>0.028120497475949</v>
+      </c>
+      <c r="AX142">
+        <v>0.036206846666419</v>
+      </c>
+      <c r="AY142">
+        <v>0.027667923969352</v>
+      </c>
+      <c r="AZ142">
+        <v>0.066621531486415</v>
+      </c>
+      <c r="BA142">
+        <v>0.042438576072111</v>
+      </c>
+      <c r="BB142">
+        <v>0.030463584164268</v>
+      </c>
+      <c r="BC142">
+        <v>0.026926259236616</v>
+      </c>
+      <c r="BD142">
+        <v>0.031136876293148</v>
+      </c>
+      <c r="BE142">
+        <v>0.032041207788852</v>
+      </c>
     </row>
     <row r="143" spans="1:57">
       <c r="A143" t="s">
         <v>197</v>
       </c>
+      <c r="B143">
+        <v>0.036056626995957</v>
+      </c>
+      <c r="C143">
+        <v>0.019230936498484</v>
+      </c>
+      <c r="D143">
+        <v>0.018555823728802</v>
+      </c>
+      <c r="F143">
+        <v>0.024298129605828</v>
+      </c>
+      <c r="G143">
+        <v>0.031793475103055</v>
+      </c>
+      <c r="H143">
+        <v>0.0342067144306</v>
+      </c>
+      <c r="I143">
+        <v>0.02969015341128</v>
+      </c>
+      <c r="J143">
+        <v>0.040615362981013</v>
+      </c>
+      <c r="K143">
+        <v>0.02738169232238</v>
+      </c>
+      <c r="L143">
+        <v>0.021071386095633</v>
+      </c>
+      <c r="M143">
+        <v>0.017916893467923</v>
+      </c>
+      <c r="N143">
+        <v>0.055823784415261</v>
+      </c>
+      <c r="O143">
+        <v>0.022575932205389</v>
+      </c>
+      <c r="P143">
+        <v>0.023461867029098</v>
+      </c>
+      <c r="Q143">
+        <v>0.025549442976806</v>
+      </c>
+      <c r="R143">
+        <v>0.023688522204234</v>
+      </c>
+      <c r="S143">
+        <v>0.024140459543457</v>
+      </c>
+      <c r="T143">
+        <v>0.025441178612249</v>
+      </c>
+      <c r="U143">
+        <v>0.026792363688514</v>
+      </c>
+      <c r="V143">
+        <v>0.030813649635585</v>
+      </c>
+      <c r="W143">
+        <v>0.037062448354945</v>
+      </c>
+      <c r="X143">
+        <v>0.029637672820225</v>
+      </c>
+      <c r="Y143">
+        <v>0.038443556365334</v>
+      </c>
+      <c r="Z143">
+        <v>0.030156466804097</v>
+      </c>
+      <c r="AA143">
+        <v>0.025383113742874</v>
+      </c>
+      <c r="AB143">
+        <v>0.02267303057277</v>
+      </c>
+      <c r="AC143">
+        <v>0.15775941230487</v>
+      </c>
+      <c r="AD143">
+        <v>0.021941769576386</v>
+      </c>
+      <c r="AE143">
+        <v>0.032496850767402</v>
+      </c>
+      <c r="AF143">
+        <v>0.021259694528061</v>
+      </c>
+      <c r="AG143">
+        <v>0.025606724721009</v>
+      </c>
+      <c r="AH143">
+        <v>0.020866341018124</v>
+      </c>
+      <c r="AI143">
+        <v>0.023098554124088</v>
+      </c>
+      <c r="AJ143">
+        <v>0.022048253478876</v>
+      </c>
+      <c r="AK143">
+        <v>0.031332898907621</v>
+      </c>
+      <c r="AL143">
+        <v>0.025927254626009</v>
+      </c>
+      <c r="AM143">
+        <v>0.029977408216543</v>
+      </c>
+      <c r="AN143">
+        <v>0.026072338210347</v>
+      </c>
+      <c r="AO143">
+        <v>0.022073512132087</v>
+      </c>
+      <c r="AP143">
+        <v>0.028389565933227</v>
+      </c>
+      <c r="AQ143">
+        <v>0.027842812306367</v>
+      </c>
+      <c r="AR143">
+        <v>0.03765735864364</v>
+      </c>
+      <c r="AS143">
+        <v>0.03277150358492</v>
+      </c>
+      <c r="AT143">
+        <v>0.022049367407069</v>
+      </c>
+      <c r="AU143">
+        <v>0.025877936618917</v>
+      </c>
+      <c r="AV143">
+        <v>0.02139342040141</v>
+      </c>
+      <c r="AW143">
+        <v>0.020963056806984</v>
+      </c>
+      <c r="AX143">
+        <v>0.027388837343561</v>
+      </c>
+      <c r="AY143">
+        <v>0.024421572423777</v>
+      </c>
+      <c r="AZ143">
+        <v>0.064813882080115</v>
+      </c>
+      <c r="BA143">
+        <v>0.036498511667059</v>
+      </c>
+      <c r="BB143">
+        <v>0.026390082159578</v>
+      </c>
+      <c r="BC143">
+        <v>0.025984305483654</v>
+      </c>
+      <c r="BD143">
+        <v>0.028652531348676</v>
+      </c>
+      <c r="BE143">
+        <v>0.031932695007861</v>
+      </c>
     </row>
     <row r="144" spans="1:57">
       <c r="A144" t="s">
         <v>198</v>
       </c>
+      <c r="B144">
+        <v>0.048123760990395</v>
+      </c>
+      <c r="C144">
+        <v>0.053739874176502</v>
+      </c>
+      <c r="D144">
+        <v>0.055470797580494</v>
+      </c>
+      <c r="F144">
+        <v>0.045716169061742</v>
+      </c>
+      <c r="G144">
+        <v>0.05035965681074</v>
+      </c>
+      <c r="H144">
+        <v>0.057714488520664</v>
+      </c>
+      <c r="I144">
+        <v>0.054243958487594</v>
+      </c>
+      <c r="J144">
+        <v>0.051784135576064</v>
+      </c>
+      <c r="K144">
+        <v>0.05164965445653</v>
+      </c>
+      <c r="L144">
+        <v>0.04962754553509</v>
+      </c>
+      <c r="M144">
+        <v>0.042908559070641</v>
+      </c>
+      <c r="N144">
+        <v>0.054301574161392</v>
+      </c>
+      <c r="O144">
+        <v>0.026799886344886</v>
+      </c>
+      <c r="P144">
+        <v>0.04345450919539</v>
+      </c>
+      <c r="Q144">
+        <v>0.046471455991862</v>
+      </c>
+      <c r="R144">
+        <v>0.037882608495981</v>
+      </c>
+      <c r="S144">
+        <v>0.039793204069452</v>
+      </c>
+      <c r="T144">
+        <v>0.04283571700687</v>
+      </c>
+      <c r="U144">
+        <v>0.042860736290548</v>
+      </c>
+      <c r="V144">
+        <v>0.051413016166666</v>
+      </c>
+      <c r="W144">
+        <v>0.044340635516918</v>
+      </c>
+      <c r="X144">
+        <v>0.042122818514873</v>
+      </c>
+      <c r="Y144">
+        <v>0.047794547920996</v>
+      </c>
+      <c r="Z144">
+        <v>0.045304779882647</v>
+      </c>
+      <c r="AA144">
+        <v>0.04314894301446</v>
+      </c>
+      <c r="AB144">
+        <v>0.047363963216755</v>
+      </c>
+      <c r="AC144">
+        <v>0.12570546737213</v>
+      </c>
+      <c r="AD144">
+        <v>0.050117715942392</v>
+      </c>
+      <c r="AE144">
+        <v>0.050635379519505</v>
+      </c>
+      <c r="AF144">
+        <v>0.046162040085153</v>
+      </c>
+      <c r="AG144">
+        <v>0.046448227784393</v>
+      </c>
+      <c r="AH144">
+        <v>0.044245463219322</v>
+      </c>
+      <c r="AI144">
+        <v>0.043405021809392</v>
+      </c>
+      <c r="AJ144">
+        <v>0.039471647122889</v>
+      </c>
+      <c r="AK144">
+        <v>0.043755205715666</v>
+      </c>
+      <c r="AL144">
+        <v>0.041722240465847</v>
+      </c>
+      <c r="AM144">
+        <v>0.043369010269377</v>
+      </c>
+      <c r="AN144">
+        <v>0.04817933987074</v>
+      </c>
+      <c r="AO144">
+        <v>0.047895866444191</v>
+      </c>
+      <c r="AP144">
+        <v>0.0464139600535</v>
+      </c>
+      <c r="AQ144">
+        <v>0.047035139028857</v>
+      </c>
+      <c r="AR144">
+        <v>0.042687252216578</v>
+      </c>
+      <c r="AS144">
+        <v>0.048059942459198</v>
+      </c>
+      <c r="AT144">
+        <v>0.048144504822544</v>
+      </c>
+      <c r="AU144">
+        <v>0.048024831668515</v>
+      </c>
+      <c r="AV144">
+        <v>0.046647983725257</v>
+      </c>
+      <c r="AW144">
+        <v>0.040618645448447</v>
+      </c>
+      <c r="AX144">
+        <v>0.05246925271751</v>
+      </c>
+      <c r="AY144">
+        <v>0.041845004039869</v>
+      </c>
+      <c r="AZ144">
+        <v>0.07236457324512199</v>
+      </c>
+      <c r="BA144">
+        <v>0.048892494249771</v>
+      </c>
+      <c r="BB144">
+        <v>0.03972162912498</v>
+      </c>
+      <c r="BC144">
+        <v>0.043563622446602</v>
+      </c>
+      <c r="BD144">
+        <v>0.044046017410033</v>
+      </c>
+      <c r="BE144">
+        <v>0.042197852599821</v>
+      </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:57">
       <c r="A145" t="s">
         <v>199</v>
       </c>
+      <c r="B145">
+        <v>0.046896382766297</v>
+      </c>
+      <c r="C145">
+        <v>0.054303385421893</v>
+      </c>
+      <c r="D145">
+        <v>0.047957802514487</v>
+      </c>
+      <c r="F145">
+        <v>0.039738625701498</v>
+      </c>
+      <c r="G145">
+        <v>0.048699917016141</v>
+      </c>
+      <c r="H145">
+        <v>0.051678195560628</v>
+      </c>
+      <c r="I145">
+        <v>0.049682723991012</v>
+      </c>
+      <c r="J145">
+        <v>0.047435220045364</v>
+      </c>
+      <c r="K145">
+        <v>0.050175029521969</v>
+      </c>
+      <c r="L145">
+        <v>0.050554909843013</v>
+      </c>
+      <c r="M145">
+        <v>0.045759049489351</v>
+      </c>
+      <c r="N145">
+        <v>0.052112270784191</v>
+      </c>
+      <c r="O145">
+        <v>0.02931796859684</v>
+      </c>
+      <c r="P145">
+        <v>0.047744931606643</v>
+      </c>
+      <c r="Q145">
+        <v>0.04974304363707</v>
+      </c>
+      <c r="R145">
+        <v>0.041253961988246</v>
+      </c>
+      <c r="S145">
+        <v>0.044713414959521</v>
+      </c>
+      <c r="T145">
+        <v>0.047329470994646</v>
+      </c>
+      <c r="U145">
+        <v>0.047614169060071</v>
+      </c>
+      <c r="V145">
+        <v>0.054279417309461</v>
+      </c>
+      <c r="W145">
+        <v>0.0511941225709</v>
+      </c>
+      <c r="X145">
+        <v>0.046729728083098</v>
+      </c>
+      <c r="Y145">
+        <v>0.056506423831414</v>
+      </c>
+      <c r="Z145">
+        <v>0.054021574899061</v>
+      </c>
+      <c r="AA145">
+        <v>0.051586222985068</v>
+      </c>
+      <c r="AB145">
+        <v>0.056220739820777</v>
+      </c>
+      <c r="AC145">
+        <v>0.10441820084677</v>
+      </c>
+      <c r="AD145">
+        <v>0.058362699673999</v>
+      </c>
+      <c r="AE145">
+        <v>0.063145004829713</v>
+      </c>
+      <c r="AF145">
+        <v>0.043129588168868</v>
+      </c>
+      <c r="AG145">
+        <v>0.042962236757504</v>
+      </c>
+      <c r="AH145">
+        <v>0.054016024239666</v>
+      </c>
+      <c r="AI145">
+        <v>0.053081861711345</v>
+      </c>
+      <c r="AJ145">
+        <v>0.045919682198461</v>
+      </c>
+      <c r="AK145">
+        <v>0.048218099456081</v>
+      </c>
+      <c r="AL145">
+        <v>0.050265321757492</v>
+      </c>
+      <c r="AM145">
+        <v>0.043760918425718</v>
+      </c>
+      <c r="AN145">
+        <v>0.042737550518508</v>
+      </c>
+      <c r="AO145">
+        <v>0.045955303941521</v>
+      </c>
+      <c r="AP145">
+        <v>0.043113341095123</v>
+      </c>
+      <c r="AQ145">
+        <v>0.044157411815978</v>
+      </c>
+      <c r="AR145">
+        <v>0.050234494610666</v>
+      </c>
+      <c r="AS145">
+        <v>0.046903105238658</v>
+      </c>
+      <c r="AT145">
+        <v>0.047252243926823</v>
+      </c>
+      <c r="AU145">
+        <v>0.050843952195806</v>
+      </c>
+      <c r="AV145">
+        <v>0.046761841191643</v>
+      </c>
+      <c r="AW145">
+        <v>0.041958681868717</v>
+      </c>
+      <c r="AX145">
+        <v>0.05678131588211</v>
+      </c>
+      <c r="AY145">
+        <v>0.0464897945357</v>
+      </c>
+      <c r="AZ145">
+        <v>0.08832363935146501</v>
+      </c>
+      <c r="BA145">
+        <v>0.056376276856167</v>
+      </c>
+      <c r="BB145">
+        <v>0.04589313621221</v>
+      </c>
+      <c r="BC145">
+        <v>0.05068029870068</v>
+      </c>
+      <c r="BD145">
+        <v>0.055429968513164</v>
+      </c>
+      <c r="BE145">
+        <v>0.051994399237294</v>
+      </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:57">
       <c r="A146" t="s">
         <v>200</v>
       </c>
+      <c r="B146">
+        <v>0.049998305473856</v>
+      </c>
+      <c r="C146">
+        <v>0.047795049721616</v>
+      </c>
+      <c r="D146">
+        <v>0.044156436952679</v>
+      </c>
+      <c r="F146">
+        <v>0.041117595622698</v>
+      </c>
+      <c r="G146">
+        <v>0.04198686664965</v>
+      </c>
+      <c r="H146">
+        <v>0.048804558465863</v>
+      </c>
+      <c r="I146">
+        <v>0.044685836334695</v>
+      </c>
+      <c r="J146">
+        <v>0.042080939547661</v>
+      </c>
+      <c r="K146">
+        <v>0.048453900103063</v>
+      </c>
+      <c r="L146">
+        <v>0.049897953313753</v>
+      </c>
+      <c r="M146">
+        <v>0.046664347694675</v>
+      </c>
+      <c r="N146">
+        <v>0.049509149422699</v>
+      </c>
+      <c r="O146">
+        <v>0.030662221267047</v>
+      </c>
+      <c r="P146">
+        <v>0.045895376862908</v>
+      </c>
+      <c r="Q146">
+        <v>0.04957677215905</v>
+      </c>
+      <c r="R146">
+        <v>0.039095606055376</v>
+      </c>
+      <c r="S146">
+        <v>0.041384390078809</v>
+      </c>
+      <c r="T146">
+        <v>0.046525231807236</v>
+      </c>
+      <c r="U146">
+        <v>0.046243229197607</v>
+      </c>
+      <c r="V146">
+        <v>0.054711600624181</v>
+      </c>
+      <c r="W146">
+        <v>0.045381235897603</v>
+      </c>
+      <c r="X146">
+        <v>0.044496030222598</v>
+      </c>
+      <c r="Y146">
+        <v>0.050162666958164</v>
+      </c>
+      <c r="Z146">
+        <v>0.046195851452297</v>
+      </c>
+      <c r="AA146">
+        <v>0.042170395216632</v>
+      </c>
+      <c r="AB146">
+        <v>0.049241574014634</v>
+      </c>
+      <c r="AC146">
+        <v>0.14048340548341</v>
+      </c>
+      <c r="AD146">
+        <v>0.051443032933084</v>
+      </c>
+      <c r="AE146">
+        <v>0.055973707438873</v>
+      </c>
+      <c r="AF146">
+        <v>0.050332929799354</v>
+      </c>
+      <c r="AG146">
+        <v>0.05097178046828</v>
+      </c>
+      <c r="AH146">
+        <v>0.048323029352111</v>
+      </c>
+      <c r="AI146">
+        <v>0.047921832604434</v>
+      </c>
+      <c r="AJ146">
+        <v>0.044131076327295</v>
+      </c>
+      <c r="AK146">
+        <v>0.050614800322697</v>
+      </c>
+      <c r="AL146">
+        <v>0.044759798872832</v>
+      </c>
+      <c r="AM146">
+        <v>0.049612764208363</v>
+      </c>
+      <c r="AN146">
+        <v>0.052544503238651</v>
+      </c>
+      <c r="AO146">
+        <v>0.053078019268807</v>
+      </c>
+      <c r="AP146">
+        <v>0.050861208162748</v>
+      </c>
+      <c r="AQ146">
+        <v>0.04990490541234</v>
+      </c>
+      <c r="AR146">
+        <v>0.046595146070184</v>
+      </c>
+      <c r="AS146">
+        <v>0.048517632094235</v>
+      </c>
+      <c r="AT146">
+        <v>0.049166049023988</v>
+      </c>
+      <c r="AU146">
+        <v>0.049741275751723</v>
+      </c>
+      <c r="AV146">
+        <v>0.046903125456679</v>
+      </c>
+      <c r="AW146">
+        <v>0.040504407385672</v>
+      </c>
+      <c r="AX146">
+        <v>0.051174621815248</v>
+      </c>
+      <c r="AY146">
+        <v>0.042059587310249</v>
+      </c>
+      <c r="AZ146">
+        <v>0.068855750204332</v>
+      </c>
+      <c r="BA146">
+        <v>0.048595571624333</v>
+      </c>
+      <c r="BB146">
+        <v>0.040020380207479</v>
+      </c>
+      <c r="BC146">
+        <v>0.043897089840386</v>
+      </c>
+      <c r="BD146">
+        <v>0.047771591755338</v>
+      </c>
+      <c r="BE146">
+        <v>0.044843668997148</v>
+      </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:57">
       <c r="A147" t="s">
         <v>201</v>
       </c>
+      <c r="B147">
+        <v>0.044789411024381</v>
+      </c>
+      <c r="C147">
+        <v>0.049599297704935</v>
+      </c>
+      <c r="D147">
+        <v>0.04994963394397</v>
+      </c>
+      <c r="F147">
+        <v>0.040840995781928</v>
+      </c>
+      <c r="G147">
+        <v>0.050204242579856</v>
+      </c>
+      <c r="H147">
+        <v>0.04501492752854</v>
+      </c>
+      <c r="I147">
+        <v>0.040783514954636</v>
+      </c>
+      <c r="J147">
+        <v>0.043717856316166</v>
+      </c>
+      <c r="K147">
+        <v>0.040237539174621</v>
+      </c>
+      <c r="L147">
+        <v>0.044515028460272</v>
+      </c>
+      <c r="M147">
+        <v>0.041807568875155</v>
+      </c>
+      <c r="N147">
+        <v>0.053295265899395</v>
+      </c>
+      <c r="O147">
+        <v>0.027243446108049</v>
+      </c>
+      <c r="P147">
+        <v>0.041710709299689</v>
+      </c>
+      <c r="Q147">
+        <v>0.047237663660281</v>
+      </c>
+      <c r="R147">
+        <v>0.038158694019685</v>
+      </c>
+      <c r="S147">
+        <v>0.041427116449925</v>
+      </c>
+      <c r="T147">
+        <v>0.0440133743068</v>
+      </c>
+      <c r="U147">
+        <v>0.043007857312962</v>
+      </c>
+      <c r="V147">
+        <v>0.050244049337324</v>
+      </c>
+      <c r="W147">
+        <v>0.043596181667891</v>
+      </c>
+      <c r="X147">
+        <v>0.041418672820872</v>
+      </c>
+      <c r="Y147">
+        <v>0.047726508743885</v>
+      </c>
+      <c r="Z147">
+        <v>0.04326716227282</v>
+      </c>
+      <c r="AA147">
+        <v>0.040017560471134</v>
+      </c>
+      <c r="AB147">
+        <v>0.049340808135737</v>
+      </c>
+      <c r="AC147">
+        <v>0.14520169846257</v>
+      </c>
+      <c r="AD147">
+        <v>0.050132497258961</v>
+      </c>
+      <c r="AE147">
+        <v>0.058993690270124</v>
+      </c>
+      <c r="AF147">
+        <v>0.049309833318681</v>
+      </c>
+      <c r="AG147">
+        <v>0.049502264231802</v>
+      </c>
+      <c r="AH147">
+        <v>0.047755625998127</v>
+      </c>
+      <c r="AI147">
+        <v>0.050259733709157</v>
+      </c>
+      <c r="AJ147">
+        <v>0.046447837701747</v>
+      </c>
+      <c r="AK147">
+        <v>0.051765017691717</v>
+      </c>
+      <c r="AL147">
+        <v>0.045857723654808</v>
+      </c>
+      <c r="AM147">
+        <v>0.050618539435646</v>
+      </c>
+      <c r="AN147">
+        <v>0.050449505294427</v>
+      </c>
+      <c r="AO147">
+        <v>0.050585375681367</v>
+      </c>
+      <c r="AP147">
+        <v>0.048925878169811</v>
+      </c>
+      <c r="AQ147">
+        <v>0.050483472362376</v>
+      </c>
+      <c r="AR147">
+        <v>0.04532191111178</v>
+      </c>
+      <c r="AS147">
+        <v>0.052224165648447</v>
+      </c>
+      <c r="AT147">
+        <v>0.051686433958382</v>
+      </c>
+      <c r="AU147">
+        <v>0.050251787600313</v>
+      </c>
+      <c r="AV147">
+        <v>0.05016091880095</v>
+      </c>
+      <c r="AW147">
+        <v>0.045453289260716</v>
+      </c>
+      <c r="AX147">
+        <v>0.057252501328213</v>
+      </c>
+      <c r="AY147">
+        <v>0.047120061230856</v>
+      </c>
+      <c r="AZ147">
+        <v>0.067806019004329</v>
+      </c>
+      <c r="BA147">
+        <v>0.053994762952816</v>
+      </c>
+      <c r="BB147">
+        <v>0.044642930527514</v>
+      </c>
+      <c r="BC147">
+        <v>0.04691182940966</v>
+      </c>
+      <c r="BD147">
+        <v>0.051255995538296</v>
+      </c>
+      <c r="BE147">
+        <v>0.043994302349993</v>
+      </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:57">
       <c r="A148" t="s">
         <v>202</v>
+      </c>
+      <c r="B148">
+        <v>0.062849348809766</v>
+      </c>
+      <c r="C148">
+        <v>0.050251442895284</v>
+      </c>
+      <c r="D148">
+        <v>0.048383613374988</v>
+      </c>
+      <c r="F148">
+        <v>0.044682724534105</v>
+      </c>
+      <c r="G148">
+        <v>0.052210035440012</v>
+      </c>
+      <c r="H148">
+        <v>0.051116689084564</v>
+      </c>
+      <c r="I148">
+        <v>0.04693705295365</v>
+      </c>
+      <c r="J148">
+        <v>0.044843451376712</v>
+      </c>
+      <c r="K148">
+        <v>0.045297200697298</v>
+      </c>
+      <c r="L148">
+        <v>0.042120726632364</v>
+      </c>
+      <c r="M148">
+        <v>0.036873503695475</v>
+      </c>
+      <c r="N148">
+        <v>0.056568981029138</v>
+      </c>
+      <c r="O148">
+        <v>0.027902047562699</v>
+      </c>
+      <c r="P148">
+        <v>0.037560756013876</v>
+      </c>
+      <c r="Q148">
+        <v>0.042014004724214</v>
+      </c>
+      <c r="R148">
+        <v>0.037610812250943</v>
+      </c>
+      <c r="S148">
+        <v>0.03673422533593</v>
+      </c>
+      <c r="T148">
+        <v>0.037098639133363</v>
+      </c>
+      <c r="U148">
+        <v>0.037240233602544</v>
+      </c>
+      <c r="V148">
+        <v>0.042811435054392</v>
+      </c>
+      <c r="W148">
+        <v>0.040339242652318</v>
+      </c>
+      <c r="X148">
+        <v>0.037238320716204</v>
+      </c>
+      <c r="Y148">
+        <v>0.040320944333015</v>
+      </c>
+      <c r="Z148">
+        <v>0.039043788617824</v>
+      </c>
+      <c r="AA148">
+        <v>0.037341779402913</v>
+      </c>
+      <c r="AB148">
+        <v>0.044348735516811</v>
+      </c>
+      <c r="AC148">
+        <v>0.12305666555667</v>
+      </c>
+      <c r="AD148">
+        <v>0.044928927543884</v>
+      </c>
+      <c r="AE148">
+        <v>0.052799868034522</v>
+      </c>
+      <c r="AF148">
+        <v>0.039031435147314</v>
+      </c>
+      <c r="AG148">
+        <v>0.04031513251019</v>
+      </c>
+      <c r="AH148">
+        <v>0.043217220159883</v>
+      </c>
+      <c r="AI148">
+        <v>0.044749023116649</v>
+      </c>
+      <c r="AJ148">
+        <v>0.04120922368748</v>
+      </c>
+      <c r="AK148">
+        <v>0.045126941567939</v>
+      </c>
+      <c r="AL148">
+        <v>0.043531268323464</v>
+      </c>
+      <c r="AM148">
+        <v>0.042271686964846</v>
+      </c>
+      <c r="AN148">
+        <v>0.041001010260294</v>
+      </c>
+      <c r="AO148">
+        <v>0.040024083101697</v>
+      </c>
+      <c r="AP148">
+        <v>0.040022545874454</v>
+      </c>
+      <c r="AQ148">
+        <v>0.041434783425432</v>
+      </c>
+      <c r="AR148">
+        <v>0.045687967300352</v>
+      </c>
+      <c r="AS148">
+        <v>0.042389394005417</v>
+      </c>
+      <c r="AT148">
+        <v>0.039076402315977</v>
+      </c>
+      <c r="AU148">
+        <v>0.039026849178744</v>
+      </c>
+      <c r="AV148">
+        <v>0.039895637650138</v>
+      </c>
+      <c r="AW148">
+        <v>0.037038512006435</v>
+      </c>
+      <c r="AX148">
+        <v>0.0477094560708</v>
+      </c>
+      <c r="AY148">
+        <v>0.040912216734073</v>
+      </c>
+      <c r="AZ148">
+        <v>0.07789136661201</v>
+      </c>
+      <c r="BA148">
+        <v>0.049471218684724</v>
+      </c>
+      <c r="BB148">
+        <v>0.041040824444526</v>
+      </c>
+      <c r="BC148">
+        <v>0.042425170046754</v>
+      </c>
+      <c r="BD148">
+        <v>0.045431742751288</v>
+      </c>
+      <c r="BE148">
+        <v>0.04363440429337</v>
+      </c>
+    </row>
+    <row r="149" spans="1:57">
+      <c r="A149" t="s">
+        <v>203</v>
+      </c>
+      <c r="B149">
+        <v>0.05327204750362</v>
+      </c>
+      <c r="C149">
+        <v>0.037297642238585</v>
+      </c>
+      <c r="D149">
+        <v>0.021501032647752</v>
+      </c>
+      <c r="F149">
+        <v>0.032197947209339</v>
+      </c>
+      <c r="G149">
+        <v>0.032147056536666</v>
+      </c>
+      <c r="H149">
+        <v>0.033411603914423</v>
+      </c>
+      <c r="I149">
+        <v>0.02714752593344</v>
+      </c>
+      <c r="J149">
+        <v>0.037038062433376</v>
+      </c>
+      <c r="K149">
+        <v>0.025644851176096</v>
+      </c>
+      <c r="L149">
+        <v>0.02246177336374</v>
+      </c>
+      <c r="M149">
+        <v>0.023026285306169</v>
+      </c>
+      <c r="N149">
+        <v>0.05134672182799</v>
+      </c>
+      <c r="O149">
+        <v>0.026278074385948</v>
+      </c>
+      <c r="P149">
+        <v>0.024223383370397</v>
+      </c>
+      <c r="Q149">
+        <v>0.034164789717788</v>
+      </c>
+      <c r="R149">
+        <v>0.029683709067806</v>
+      </c>
+      <c r="S149">
+        <v>0.02559879286996</v>
+      </c>
+      <c r="T149">
+        <v>0.024421978039677</v>
+      </c>
+      <c r="U149">
+        <v>0.024439212207923</v>
+      </c>
+      <c r="V149">
+        <v>0.028492728010184</v>
+      </c>
+      <c r="W149">
+        <v>0.035720869174208</v>
+      </c>
+      <c r="X149">
+        <v>0.028507031871354</v>
+      </c>
+      <c r="Y149">
+        <v>0.033285625205329</v>
+      </c>
+      <c r="Z149">
+        <v>0.031959700198708</v>
+      </c>
+      <c r="AA149">
+        <v>0.029859855454991</v>
+      </c>
+      <c r="AB149">
+        <v>0.02987847157244</v>
+      </c>
+      <c r="AC149">
+        <v>0.1483024691358</v>
+      </c>
+      <c r="AD149">
+        <v>0.027910535252725</v>
+      </c>
+      <c r="AE149">
+        <v>0.041007664901499</v>
+      </c>
+      <c r="AF149">
+        <v>0.025087252884791</v>
+      </c>
+      <c r="AG149">
+        <v>0.028710952675836</v>
+      </c>
+      <c r="AH149">
+        <v>0.029529476163507</v>
+      </c>
+      <c r="AI149">
+        <v>0.031451868780839</v>
+      </c>
+      <c r="AJ149">
+        <v>0.031341237765197</v>
+      </c>
+      <c r="AK149">
+        <v>0.039234782749548</v>
+      </c>
+      <c r="AL149">
+        <v>0.035496925348758</v>
+      </c>
+      <c r="AM149">
+        <v>0.035112618369289</v>
+      </c>
+      <c r="AN149">
+        <v>0.027376381835185</v>
+      </c>
+      <c r="AO149">
+        <v>0.025959773088824</v>
+      </c>
+      <c r="AP149">
+        <v>0.032500225136832</v>
+      </c>
+      <c r="AQ149">
+        <v>0.032071948527627</v>
+      </c>
+      <c r="AR149">
+        <v>0.038667220608031</v>
+      </c>
+      <c r="AS149">
+        <v>0.036300807583484</v>
+      </c>
+      <c r="AT149">
+        <v>0.027557992235274</v>
+      </c>
+      <c r="AU149">
+        <v>0.031684868228233</v>
+      </c>
+      <c r="AV149">
+        <v>0.026042118151536</v>
+      </c>
+      <c r="AW149">
+        <v>0.024523983216895</v>
+      </c>
+      <c r="AX149">
+        <v>0.030504584643149</v>
+      </c>
+      <c r="AY149">
+        <v>0.026069578444262</v>
+      </c>
+      <c r="AZ149">
+        <v>0.065380422824819</v>
+      </c>
+      <c r="BA149">
+        <v>0.037171433715942</v>
+      </c>
+      <c r="BB149">
+        <v>0.028263656322266</v>
+      </c>
+      <c r="BC149">
+        <v>0.02740275348527</v>
+      </c>
+      <c r="BD149">
+        <v>0.029550273457236</v>
+      </c>
+      <c r="BE149">
+        <v>0.033736257756991</v>
+      </c>
+    </row>
+    <row r="150" spans="1:57">
+      <c r="A150" t="s">
+        <v>204</v>
+      </c>
+      <c r="B150">
+        <v>0.037319010889107</v>
+      </c>
+      <c r="C150">
+        <v>0.017146743769708</v>
+      </c>
+      <c r="D150">
+        <v>0.02485851822449</v>
+      </c>
+      <c r="F150">
+        <v>0.030465502794839</v>
+      </c>
+      <c r="G150">
+        <v>0.036114290350326</v>
+      </c>
+      <c r="H150">
+        <v>0.034171044525759</v>
+      </c>
+      <c r="I150">
+        <v>0.028641192821798</v>
+      </c>
+      <c r="J150">
+        <v>0.042618699480383</v>
+      </c>
+      <c r="K150">
+        <v>0.029022440609725</v>
+      </c>
+      <c r="L150">
+        <v>0.020720344115644</v>
+      </c>
+      <c r="M150">
+        <v>0.016427767543451</v>
+      </c>
+      <c r="N150">
+        <v>0.05589949316962</v>
+      </c>
+      <c r="O150">
+        <v>0.022310797517159</v>
+      </c>
+      <c r="P150">
+        <v>0.02331057860091</v>
+      </c>
+      <c r="Q150">
+        <v>0.023958357417783</v>
+      </c>
+      <c r="R150">
+        <v>0.023430966778945</v>
+      </c>
+      <c r="S150">
+        <v>0.022397687502137</v>
+      </c>
+      <c r="T150">
+        <v>0.023339610872832</v>
+      </c>
+      <c r="U150">
+        <v>0.022541263241141</v>
+      </c>
+      <c r="V150">
+        <v>0.026242408973796</v>
+      </c>
+      <c r="W150">
+        <v>0.030055393911273</v>
+      </c>
+      <c r="X150">
+        <v>0.025003599266006</v>
+      </c>
+      <c r="Y150">
+        <v>0.031084699502902</v>
+      </c>
+      <c r="Z150">
+        <v>0.02693062928075</v>
+      </c>
+      <c r="AA150">
+        <v>0.024070286248619</v>
+      </c>
+      <c r="AB150">
+        <v>0.024089054677554</v>
+      </c>
+      <c r="AC150">
+        <v>0.12609126984127</v>
+      </c>
+      <c r="AD150">
+        <v>0.022423899941853</v>
+      </c>
+      <c r="AE150">
+        <v>0.035300084929984</v>
+      </c>
+      <c r="AF150">
+        <v>0.020691497656637</v>
+      </c>
+      <c r="AG150">
+        <v>0.024885065154945</v>
+      </c>
+      <c r="AH150">
+        <v>0.023421925396495</v>
+      </c>
+      <c r="AI150">
+        <v>0.025290640735104</v>
+      </c>
+      <c r="AJ150">
+        <v>0.025906029695742</v>
+      </c>
+      <c r="AK150">
+        <v>0.036479935514726</v>
+      </c>
+      <c r="AL150">
+        <v>0.02844203064098</v>
+      </c>
+      <c r="AM150">
+        <v>0.032034726494434</v>
+      </c>
+      <c r="AN150">
+        <v>0.024148114068378</v>
+      </c>
+      <c r="AO150">
+        <v>0.020720793543107</v>
+      </c>
+      <c r="AP150">
+        <v>0.026330788764746</v>
+      </c>
+      <c r="AQ150">
+        <v>0.02654449927284</v>
+      </c>
+      <c r="AR150">
+        <v>0.03498530855758</v>
+      </c>
+      <c r="AS150">
+        <v>0.031699964834512</v>
+      </c>
+      <c r="AT150">
+        <v>0.021687459647462</v>
+      </c>
+      <c r="AU150">
+        <v>0.027705223761368</v>
+      </c>
+      <c r="AV150">
+        <v>0.021332901841434</v>
+      </c>
+      <c r="AW150">
+        <v>0.02258298975503</v>
+      </c>
+      <c r="AX150">
+        <v>0.030498130372002</v>
+      </c>
+      <c r="AY150">
+        <v>0.027046555882961</v>
+      </c>
+      <c r="AZ150">
+        <v>0.061344753039202</v>
+      </c>
+      <c r="BA150">
+        <v>0.03942634224677</v>
+      </c>
+      <c r="BB150">
+        <v>0.030117937279241</v>
+      </c>
+      <c r="BC150">
+        <v>0.029213363471011</v>
+      </c>
+      <c r="BD150">
+        <v>0.031067267268858</v>
+      </c>
+      <c r="BE150">
+        <v>0.035126755159582</v>
+      </c>
+    </row>
+    <row r="151" spans="1:57">
+      <c r="A151" t="s">
+        <v>205</v>
+      </c>
+      <c r="B151">
+        <v>0.048876739695883</v>
+      </c>
+      <c r="C151">
+        <v>0.057478894011428</v>
+      </c>
+      <c r="D151">
+        <v>0.041813854741075</v>
+      </c>
+      <c r="F151">
+        <v>0.036552689520604</v>
+      </c>
+      <c r="G151">
+        <v>0.04893895429365</v>
+      </c>
+      <c r="H151">
+        <v>0.047460564757582</v>
+      </c>
+      <c r="I151">
+        <v>0.041319481793806</v>
+      </c>
+      <c r="J151">
+        <v>0.041868203028524</v>
+      </c>
+      <c r="K151">
+        <v>0.042365028857707</v>
+      </c>
+      <c r="L151">
+        <v>0.044263948140257</v>
+      </c>
+      <c r="M151">
+        <v>0.043434406733657</v>
+      </c>
+      <c r="N151">
+        <v>0.050099288740378</v>
+      </c>
+      <c r="O151">
+        <v>0.028784511978172</v>
+      </c>
+      <c r="P151">
+        <v>0.046493942351756</v>
+      </c>
+      <c r="Q151">
+        <v>0.049851336499033</v>
+      </c>
+      <c r="R151">
+        <v>0.040643457468354</v>
+      </c>
+      <c r="S151">
+        <v>0.042195386152695</v>
+      </c>
+      <c r="T151">
+        <v>0.04648816371004</v>
+      </c>
+      <c r="U151">
+        <v>0.046343559529607</v>
+      </c>
+      <c r="V151">
+        <v>0.055981019883015</v>
+      </c>
+      <c r="W151">
+        <v>0.053343266681177</v>
+      </c>
+      <c r="X151">
+        <v>0.049675713964585</v>
+      </c>
+      <c r="Y151">
+        <v>0.053834578844951</v>
+      </c>
+      <c r="Z151">
+        <v>0.050624226024987</v>
+      </c>
+      <c r="AA151">
+        <v>0.042925719085926</v>
+      </c>
+      <c r="AB151">
+        <v>0.048578566251394</v>
+      </c>
+      <c r="AC151">
+        <v>0.14698412698413</v>
+      </c>
+      <c r="AD151">
+        <v>0.049093332321276</v>
+      </c>
+      <c r="AE151">
+        <v>0.053658130034967</v>
+      </c>
+      <c r="AF151">
+        <v>0.042986354526828</v>
+      </c>
+      <c r="AG151">
+        <v>0.041557931333178</v>
+      </c>
+      <c r="AH151">
+        <v>0.047006600661874</v>
+      </c>
+      <c r="AI151">
+        <v>0.044166425881659</v>
+      </c>
+      <c r="AJ151">
+        <v>0.041689773378942</v>
+      </c>
+      <c r="AK151">
+        <v>0.046356876557406</v>
+      </c>
+      <c r="AL151">
+        <v>0.042493882237873</v>
+      </c>
+      <c r="AM151">
+        <v>0.044169945083959</v>
+      </c>
+      <c r="AN151">
+        <v>0.045998361212859</v>
+      </c>
+      <c r="AO151">
+        <v>0.048609622694138</v>
+      </c>
+      <c r="AP151">
+        <v>0.04825582078209</v>
+      </c>
+      <c r="AQ151">
+        <v>0.051928211160408</v>
+      </c>
+      <c r="AR151">
+        <v>0.048414463593053</v>
+      </c>
+      <c r="AS151">
+        <v>0.054908241034421</v>
+      </c>
+      <c r="AT151">
+        <v>0.051851650083726</v>
+      </c>
+      <c r="AU151">
+        <v>0.0559964277395</v>
+      </c>
+      <c r="AV151">
+        <v>0.050569406520143</v>
+      </c>
+      <c r="AW151">
+        <v>0.043166104506596</v>
+      </c>
+      <c r="AX151">
+        <v>0.056566177411495</v>
+      </c>
+      <c r="AY151">
+        <v>0.045634442523014</v>
+      </c>
+      <c r="AZ151">
+        <v>0.084744525723398</v>
+      </c>
+      <c r="BA151">
+        <v>0.055793763912721</v>
+      </c>
+      <c r="BB151">
+        <v>0.043016002713213</v>
+      </c>
+      <c r="BC151">
+        <v>0.047424180026561</v>
+      </c>
+      <c r="BD151">
+        <v>0.048551045115695</v>
+      </c>
+      <c r="BE151">
+        <v>0.047869358393565</v>
+      </c>
+    </row>
+    <row r="152" spans="1:57">
+      <c r="A152" t="s">
+        <v>206</v>
+      </c>
+      <c r="B152">
+        <v>0.05059073188479</v>
+      </c>
+      <c r="C152">
+        <v>0.056571962031844</v>
+      </c>
+      <c r="D152">
+        <v>0.046962528984649</v>
+      </c>
+      <c r="F152">
+        <v>0.043960211472176</v>
+      </c>
+      <c r="G152">
+        <v>0.048671149065085</v>
+      </c>
+      <c r="H152">
+        <v>0.053739068840112</v>
+      </c>
+      <c r="I152">
+        <v>0.049370228866672</v>
+      </c>
+      <c r="J152">
+        <v>0.051486203606871</v>
+      </c>
+      <c r="K152">
+        <v>0.050177735902817</v>
+      </c>
+      <c r="L152">
+        <v>0.052100175912247</v>
+      </c>
+      <c r="M152">
+        <v>0.04834478936098</v>
+      </c>
+      <c r="N152">
+        <v>0.052576012288668</v>
+      </c>
+      <c r="O152">
+        <v>0.03426996635676</v>
+      </c>
+      <c r="P152">
+        <v>0.0546548112281</v>
+      </c>
+      <c r="Q152">
+        <v>0.058115428866474</v>
+      </c>
+      <c r="R152">
+        <v>0.049566793579933</v>
+      </c>
+      <c r="S152">
+        <v>0.050306054085716</v>
+      </c>
+      <c r="T152">
+        <v>0.051813183839765</v>
+      </c>
+      <c r="U152">
+        <v>0.049186124070485</v>
+      </c>
+      <c r="V152">
+        <v>0.054210499550045</v>
+      </c>
+      <c r="W152">
+        <v>0.042653346049064</v>
+      </c>
+      <c r="X152">
+        <v>0.042979118258379</v>
+      </c>
+      <c r="Y152">
+        <v>0.049832790703376</v>
+      </c>
+      <c r="Z152">
+        <v>0.041823974245993</v>
+      </c>
+      <c r="AA152">
+        <v>0.038182205723772</v>
+      </c>
+      <c r="AB152">
+        <v>0.045281663871563</v>
+      </c>
+      <c r="AC152">
+        <v>0.13091075591076</v>
+      </c>
+      <c r="AD152">
+        <v>0.045891967351325</v>
+      </c>
+      <c r="AE152">
+        <v>0.051352552481309</v>
+      </c>
+      <c r="AF152">
+        <v>0.04610654250978</v>
+      </c>
+      <c r="AG152">
+        <v>0.043375544557569</v>
+      </c>
+      <c r="AH152">
+        <v>0.044336517425155</v>
+      </c>
+      <c r="AI152">
+        <v>0.043515672794412</v>
+      </c>
+      <c r="AJ152">
+        <v>0.03980901428309</v>
+      </c>
+      <c r="AK152">
+        <v>0.047294417378503</v>
+      </c>
+      <c r="AL152">
+        <v>0.040668717893289</v>
+      </c>
+      <c r="AM152">
+        <v>0.045055777888437</v>
+      </c>
+      <c r="AN152">
+        <v>0.046664149842677</v>
+      </c>
+      <c r="AO152">
+        <v>0.046416743889437</v>
+      </c>
+      <c r="AP152">
+        <v>0.045822053944669</v>
+      </c>
+      <c r="AQ152">
+        <v>0.045339954030887</v>
+      </c>
+      <c r="AR152">
+        <v>0.052771166959443</v>
+      </c>
+      <c r="AS152">
+        <v>0.045571206648737</v>
+      </c>
+      <c r="AT152">
+        <v>0.046323395379374</v>
+      </c>
+      <c r="AU152">
+        <v>0.047985380442044</v>
+      </c>
+      <c r="AV152">
+        <v>0.044758117786035</v>
+      </c>
+      <c r="AW152">
+        <v>0.040081042814237</v>
+      </c>
+      <c r="AX152">
+        <v>0.052905413771706</v>
+      </c>
+      <c r="AY152">
+        <v>0.043255838114424</v>
+      </c>
+      <c r="AZ152">
+        <v>0.087002166629364</v>
+      </c>
+      <c r="BA152">
+        <v>0.049505492620918</v>
+      </c>
+      <c r="BB152">
+        <v>0.043484856516056</v>
+      </c>
+      <c r="BC152">
+        <v>0.048068639170659</v>
+      </c>
+      <c r="BD152">
+        <v>0.047954898443884</v>
+      </c>
+      <c r="BE152">
+        <v>0.047429109388752</v>
+      </c>
+    </row>
+    <row r="153" spans="1:57">
+      <c r="A153" t="s">
+        <v>207</v>
+      </c>
+      <c r="B153">
+        <v>0.05038219721231</v>
+      </c>
+      <c r="C153">
+        <v>0.047186973937513</v>
+      </c>
+      <c r="D153">
+        <v>0.049211878585257</v>
+      </c>
+      <c r="F153">
+        <v>0.044252807782656</v>
+      </c>
+      <c r="G153">
+        <v>0.050973555225432</v>
+      </c>
+      <c r="H153">
+        <v>0.056356583580701</v>
+      </c>
+      <c r="I153">
+        <v>0.047706768582388</v>
+      </c>
+      <c r="J153">
+        <v>0.047580222272963</v>
+      </c>
+      <c r="K153">
+        <v>0.044488908773125</v>
+      </c>
+      <c r="L153">
+        <v>0.045708784781059</v>
+      </c>
+      <c r="M153">
+        <v>0.045113659786193</v>
+      </c>
+      <c r="N153">
+        <v>0.050273378268391</v>
+      </c>
+      <c r="O153">
+        <v>0.036298640837547</v>
+      </c>
+      <c r="P153">
+        <v>0.051063799021988</v>
+      </c>
+      <c r="Q153">
+        <v>0.060873688703141</v>
+      </c>
+      <c r="R153">
+        <v>0.054417025595602</v>
+      </c>
+      <c r="S153">
+        <v>0.051960897553386</v>
+      </c>
+      <c r="T153">
+        <v>0.049392801735565</v>
+      </c>
+      <c r="U153">
+        <v>0.0465105827261</v>
+      </c>
+      <c r="V153">
+        <v>0.05263850451463</v>
+      </c>
+      <c r="W153">
+        <v>0.048219189785251</v>
+      </c>
+      <c r="X153">
+        <v>0.043859560629496</v>
+      </c>
+      <c r="Y153">
+        <v>0.049394005770192</v>
+      </c>
+      <c r="Z153">
+        <v>0.051025837428431</v>
+      </c>
+      <c r="AA153">
+        <v>0.047649359412136</v>
+      </c>
+      <c r="AB153">
+        <v>0.051421123654853</v>
+      </c>
+      <c r="AC153">
+        <v>0.12097347097347</v>
+      </c>
+      <c r="AD153">
+        <v>0.054022572404807</v>
+      </c>
+      <c r="AE153">
+        <v>0.056419037984219</v>
+      </c>
+      <c r="AF153">
+        <v>0.04309886124449</v>
+      </c>
+      <c r="AG153">
+        <v>0.043937115076405</v>
+      </c>
+      <c r="AH153">
+        <v>0.04803901661793</v>
+      </c>
+      <c r="AI153">
+        <v>0.045085037454005</v>
+      </c>
+      <c r="AJ153">
+        <v>0.040896214944045</v>
+      </c>
+      <c r="AK153">
+        <v>0.045215849935915</v>
+      </c>
+      <c r="AL153">
+        <v>0.045228795867442</v>
+      </c>
+      <c r="AM153">
+        <v>0.042640332559599</v>
+      </c>
+      <c r="AN153">
+        <v>0.044601996661846</v>
+      </c>
+      <c r="AO153">
+        <v>0.045996230019874</v>
+      </c>
+      <c r="AP153">
+        <v>0.043835766601771</v>
+      </c>
+      <c r="AQ153">
+        <v>0.044394221438018</v>
+      </c>
+      <c r="AR153">
+        <v>0.04692265130908</v>
+      </c>
+      <c r="AS153">
+        <v>0.044831070925316</v>
+      </c>
+      <c r="AT153">
+        <v>0.045491595942297</v>
+      </c>
+      <c r="AU153">
+        <v>0.046499223818655</v>
+      </c>
+      <c r="AV153">
+        <v>0.043745665251753</v>
+      </c>
+      <c r="AW153">
+        <v>0.040746508149962</v>
+      </c>
+      <c r="AX153">
+        <v>0.053282024787874</v>
+      </c>
+      <c r="AY153">
+        <v>0.044895796663281</v>
+      </c>
+      <c r="AZ153">
+        <v>0.07830940943718501</v>
+      </c>
+      <c r="BA153">
+        <v>0.049653467084041</v>
+      </c>
+      <c r="BB153">
+        <v>0.045176022239154</v>
+      </c>
+      <c r="BC153">
+        <v>0.048479235777575</v>
+      </c>
+      <c r="BD153">
+        <v>0.04906765740973</v>
+      </c>
+      <c r="BE153">
+        <v>0.048727032106513</v>
+      </c>
+    </row>
+    <row r="154" spans="1:57">
+      <c r="A154" t="s">
+        <v>208</v>
+      </c>
+      <c r="B154">
+        <v>0.051844258347791</v>
+      </c>
+      <c r="C154">
+        <v>0.042563476553873</v>
+      </c>
+      <c r="D154">
+        <v>0.045811445202711</v>
+      </c>
+      <c r="F154">
+        <v>0.045526295893055</v>
+      </c>
+      <c r="G154">
+        <v>0.050467674761485</v>
+      </c>
+      <c r="H154">
+        <v>0.053379990159501</v>
+      </c>
+      <c r="I154">
+        <v>0.045532044454281</v>
+      </c>
+      <c r="J154">
+        <v>0.046625186952233</v>
+      </c>
+      <c r="K154">
+        <v>0.045632582100557</v>
+      </c>
+      <c r="L154">
+        <v>0.043309720096343</v>
+      </c>
+      <c r="M154">
+        <v>0.038303134363428</v>
+      </c>
+      <c r="N154">
+        <v>0.051519976015231</v>
+      </c>
+      <c r="O154">
+        <v>0.02952984744186</v>
+      </c>
+      <c r="P154">
+        <v>0.038091500673411</v>
+      </c>
+      <c r="Q154">
+        <v>0.044402521167002</v>
+      </c>
+      <c r="R154">
+        <v>0.038259447452816</v>
+      </c>
+      <c r="S154">
+        <v>0.037486766385801</v>
+      </c>
+      <c r="T154">
+        <v>0.03718172232468</v>
+      </c>
+      <c r="U154">
+        <v>0.03810018707207</v>
+      </c>
+      <c r="V154">
+        <v>0.044513139206428</v>
+      </c>
+      <c r="W154">
+        <v>0.038454910824141</v>
+      </c>
+      <c r="X154">
+        <v>0.03719203325682</v>
+      </c>
+      <c r="Y154">
+        <v>0.04292690811822</v>
+      </c>
+      <c r="Z154">
+        <v>0.039592194285997</v>
+      </c>
+      <c r="AA154">
+        <v>0.035451618449781</v>
+      </c>
+      <c r="AB154">
+        <v>0.041110255188814</v>
+      </c>
+      <c r="AC154">
+        <v>0.12933228387774</v>
+      </c>
+      <c r="AD154">
+        <v>0.043508789113959</v>
+      </c>
+      <c r="AE154">
+        <v>0.050384042924184</v>
+      </c>
+      <c r="AF154">
+        <v>0.041578904592729</v>
+      </c>
+      <c r="AG154">
+        <v>0.039922937158654</v>
+      </c>
+      <c r="AH154">
+        <v>0.039649957315055</v>
+      </c>
+      <c r="AI154">
+        <v>0.039482268418122</v>
+      </c>
+      <c r="AJ154">
+        <v>0.037474251742744</v>
+      </c>
+      <c r="AK154">
+        <v>0.046311516942416</v>
+      </c>
+      <c r="AL154">
+        <v>0.038243103357605</v>
+      </c>
+      <c r="AM154">
+        <v>0.044196430859188</v>
+      </c>
+      <c r="AN154">
+        <v>0.042847088506981</v>
+      </c>
+      <c r="AO154">
+        <v>0.040661257669827</v>
+      </c>
+      <c r="AP154">
+        <v>0.0413796040529</v>
+      </c>
+      <c r="AQ154">
+        <v>0.041944803334487</v>
+      </c>
+      <c r="AR154">
+        <v>0.049549674021401</v>
+      </c>
+      <c r="AS154">
+        <v>0.042307521052917</v>
+      </c>
+      <c r="AT154">
+        <v>0.041465529807153</v>
+      </c>
+      <c r="AU154">
+        <v>0.043496840863199</v>
+      </c>
+      <c r="AV154">
+        <v>0.041229055962384</v>
+      </c>
+      <c r="AW154">
+        <v>0.03807787993332</v>
+      </c>
+      <c r="AX154">
+        <v>0.04922335560939</v>
+      </c>
+      <c r="AY154">
+        <v>0.041157598134841</v>
+      </c>
+      <c r="AZ154">
+        <v>0.07737806324975301</v>
+      </c>
+      <c r="BA154">
+        <v>0.052630043092029</v>
+      </c>
+      <c r="BB154">
+        <v>0.041899913419022</v>
+      </c>
+      <c r="BC154">
+        <v>0.043011430297458</v>
+      </c>
+      <c r="BD154">
+        <v>0.046124784961397</v>
+      </c>
+      <c r="BE154">
+        <v>0.046031260915208</v>
+      </c>
+    </row>
+    <row r="155" spans="1:57">
+      <c r="A155" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="156" spans="1:57">
+      <c r="A156" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="157" spans="1:57">
+      <c r="A157" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="158" spans="1:57">
+      <c r="A158" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="159" spans="1:57">
+      <c r="A159" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>